<commit_message>
Solucionamos que cada usuario pueda tener más de 1 mail en la celda
</commit_message>
<xml_diff>
--- a/TallerII/datos2.xlsx
+++ b/TallerII/datos2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\GitHub\TallerII\TallerII\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2D9B47-BDB6-4F5B-926D-0686B11DE5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="45" windowWidth="9480" windowHeight="10403"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="169">
   <si>
     <t>Ejemplares : Retrasos por usuario</t>
   </si>
@@ -500,13 +506,34 @@
   </si>
   <si>
     <t>lula@gmail.com</t>
+  </si>
+  <si>
+    <t>Leites Urioste</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Mistborn</t>
+  </si>
+  <si>
+    <t>pedroleitesu2004@gmail.com        leitespsinsajo@gmail.com</t>
+  </si>
+  <si>
+    <t>Percy Jackson 5</t>
+  </si>
+  <si>
+    <t>El Eternauta</t>
+  </si>
+  <si>
+    <t>El silencio de los turnos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -516,6 +543,11 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -545,17 +577,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{AF2409AF-0377-4F2D-BF71-703E948233D3}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -628,6 +689,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -675,7 +739,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -708,9 +772,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -743,6 +824,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -918,37 +1016,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" customWidth="1"/>
-    <col min="3" max="3" width="6.73046875" customWidth="1"/>
-    <col min="5" max="5" width="22.9296875" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" customWidth="1"/>
-    <col min="7" max="7" width="48.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.19921875" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.9296875" customWidth="1"/>
-    <col min="11" max="11" width="6.86328125" customWidth="1"/>
-    <col min="12" max="12" width="9.796875" customWidth="1"/>
-    <col min="13" max="13" width="5.53125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="52.5703125" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="57.19921875" customWidth="1"/>
+    <col min="15" max="15" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1001,7 +1099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1054,7 +1152,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1205,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1160,7 +1258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1213,7 +1311,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1266,7 +1364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1319,7 +1417,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1372,7 +1470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1425,7 +1523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1478,7 +1576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1531,7 +1629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1584,7 +1682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -1637,7 +1735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1690,7 +1788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -1743,7 +1841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1796,7 +1894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1849,7 +1947,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1902,7 +2000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1955,7 +2053,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -2008,7 +2106,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -2061,7 +2159,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2114,7 +2212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -2167,7 +2265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -2220,7 +2318,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -2273,7 +2371,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -2326,7 +2424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -2379,7 +2477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -2432,7 +2530,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -2485,7 +2583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2538,7 +2636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2591,32 +2689,236 @@
         <v>22</v>
       </c>
     </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>144</v>
+      </c>
+      <c r="E34" t="s">
+        <v>162</v>
+      </c>
+      <c r="F34" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34">
+        <v>144</v>
+      </c>
+      <c r="I34">
+        <v>54554334</v>
+      </c>
+      <c r="J34" t="s">
+        <v>118</v>
+      </c>
+      <c r="K34">
+        <v>101</v>
+      </c>
+      <c r="L34">
+        <v>404</v>
+      </c>
+      <c r="M34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34">
+        <v>404</v>
+      </c>
+      <c r="O34" t="s">
+        <v>164</v>
+      </c>
+      <c r="P34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>144</v>
+      </c>
+      <c r="E35" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H35">
+        <v>144</v>
+      </c>
+      <c r="I35">
+        <v>54554334</v>
+      </c>
+      <c r="J35" t="s">
+        <v>118</v>
+      </c>
+      <c r="K35">
+        <v>102</v>
+      </c>
+      <c r="L35">
+        <v>404</v>
+      </c>
+      <c r="M35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35">
+        <v>404</v>
+      </c>
+      <c r="O35" t="s">
+        <v>166</v>
+      </c>
+      <c r="P35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>144</v>
+      </c>
+      <c r="E36" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H36">
+        <v>144</v>
+      </c>
+      <c r="I36">
+        <v>54554334</v>
+      </c>
+      <c r="J36" t="s">
+        <v>118</v>
+      </c>
+      <c r="K36">
+        <v>103</v>
+      </c>
+      <c r="L36">
+        <v>404</v>
+      </c>
+      <c r="M36" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36">
+        <v>404</v>
+      </c>
+      <c r="O36" t="s">
+        <v>167</v>
+      </c>
+      <c r="P36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>144</v>
+      </c>
+      <c r="E37" t="s">
+        <v>162</v>
+      </c>
+      <c r="F37" t="s">
+        <v>163</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H37">
+        <v>144</v>
+      </c>
+      <c r="I37">
+        <v>54554334</v>
+      </c>
+      <c r="J37" t="s">
+        <v>118</v>
+      </c>
+      <c r="K37">
+        <v>104</v>
+      </c>
+      <c r="L37">
+        <v>404</v>
+      </c>
+      <c r="M37" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37">
+        <v>404</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="P37" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G11" r:id="rId1"/>
-    <hyperlink ref="G12" r:id="rId2"/>
-    <hyperlink ref="G16" r:id="rId3"/>
-    <hyperlink ref="G9" r:id="rId4"/>
-    <hyperlink ref="G10" r:id="rId5"/>
-    <hyperlink ref="G14" r:id="rId6"/>
-    <hyperlink ref="G15" r:id="rId7"/>
-    <hyperlink ref="G17:G18" r:id="rId8" display="manuelmanuel@gmail.com"/>
-    <hyperlink ref="G19" r:id="rId9"/>
-    <hyperlink ref="G20" r:id="rId10"/>
-    <hyperlink ref="G21" r:id="rId11"/>
-    <hyperlink ref="G22" r:id="rId12"/>
-    <hyperlink ref="G23" r:id="rId13"/>
-    <hyperlink ref="G24" r:id="rId14"/>
-    <hyperlink ref="G25:G27" r:id="rId15" display="analopez@gmail.com"/>
-    <hyperlink ref="G28" r:id="rId16"/>
-    <hyperlink ref="G33" r:id="rId17"/>
-    <hyperlink ref="G29" r:id="rId18"/>
-    <hyperlink ref="G30:G31" r:id="rId19" display="juan1968@gmail.com"/>
-    <hyperlink ref="G5" r:id="rId20"/>
+    <hyperlink ref="G11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G17:G18" r:id="rId8" display="manuelmanuel@gmail.com" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G21" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G22" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G23" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G24" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G25:G27" r:id="rId15" display="analopez@gmail.com" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G33" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G29" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G30:G31" r:id="rId19" display="juan1968@gmail.com" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G5" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G34" r:id="rId21" display="pedroleitesu2004@gmail.com" xr:uid="{01F59296-DBB5-4F06-9A3E-0EE38D0DA95F}"/>
+    <hyperlink ref="G35" r:id="rId22" display="pedroleitesu2004@gmail.com" xr:uid="{6F3B89A1-5A27-41D6-987B-9685E2181AA9}"/>
+    <hyperlink ref="G37" r:id="rId23" display="pedroleitesu2004@gmail.com" xr:uid="{1A0B1D89-75DC-4A4E-A4BD-51A87875EB3C}"/>
+    <hyperlink ref="G36" r:id="rId24" display="pedroleitesu2004@gmail.com" xr:uid="{D8C46096-799B-4ACA-ADA0-4465E85E066D}"/>
   </hyperlinks>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId25"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>